<commit_message>
Start generation log for ibkIltis and update setup instructions
</commit_message>
<xml_diff>
--- a/_workingFolder/CFBData/GenerationLog.xlsx
+++ b/_workingFolder/CFBData/GenerationLog.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuhnso\Documents\GitHub\StructuralEvaluationOfCFB\_workingFolder\CFBData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACAB0BB-1A6E-4C24-A660-39337B489358}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B045D292-BE96-4330-AB04-65B41E96832B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" xr2:uid="{13CAE3C4-3EF5-4EF3-84E6-2C4B09A97B5A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" activeTab="1" xr2:uid="{13CAE3C4-3EF5-4EF3-84E6-2C4B09A97B5A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ibkGuerza" sheetId="1" r:id="rId1"/>
+    <sheet name="ibkIltis" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
   <si>
     <t>Generation Log</t>
   </si>
@@ -511,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D4357F-5063-4EF7-AA12-B87B4765B76C}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -962,4 +963,364 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF7442-AE2A-41D1-AC75-AC2A4CC2EA55}">
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>501</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>130</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>140</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>150</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update generation log and Setup instructions
</commit_message>
<xml_diff>
--- a/_workingFolder/CFBData/GenerationLog.xlsx
+++ b/_workingFolder/CFBData/GenerationLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuhnso\Documents\GitHub\StructuralEvaluationOfCFB\_workingFolder\CFBData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B045D292-BE96-4330-AB04-65B41E96832B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761C166D-E85D-4C3D-A896-BD60DE25F440}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" activeTab="1" xr2:uid="{13CAE3C4-3EF5-4EF3-84E6-2C4B09A97B5A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>Generation Log</t>
   </si>
@@ -137,6 +137,36 @@
   </si>
   <si>
     <t>….</t>
+  </si>
+  <si>
+    <t>GenStatus</t>
+  </si>
+  <si>
+    <t>CalcStatus</t>
+  </si>
+  <si>
+    <t>PostStatus</t>
+  </si>
+  <si>
+    <t>Hero Parameters (fsu_fac=1.08)</t>
+  </si>
+  <si>
+    <t>t_p (200-1200)</t>
+  </si>
+  <si>
+    <t>Hero Parameters (but L=15000,  fsu_fac=1.08)</t>
+  </si>
+  <si>
+    <t>Hero Parameters (but L=8000, fsu_fac=1.08)</t>
+  </si>
+  <si>
+    <t>t_w (200-1200)</t>
+  </si>
+  <si>
+    <t>L (2000,18000)</t>
+  </si>
+  <si>
+    <t>Hero Parameters (fsu_fac=1.08, d1/4=30, d3=20, t_p=600)</t>
   </si>
 </sst>
 </file>
@@ -967,23 +997,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF7442-AE2A-41D1-AC75-AC2A4CC2EA55}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1000,10 +1031,16 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>501</v>
       </c>
@@ -1019,10 +1056,13 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>10</v>
+        <v>510</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1036,67 +1076,73 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
+        <v>520</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>21</v>
+        <v>521</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>22</v>
+        <v>522</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1105,218 +1151,235 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
+        <v>540</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>541</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>60</v>
       </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
         <v>17</v>
       </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
         <v>18</v>
       </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>80</v>
       </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
         <v>19</v>
       </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25">
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>90</v>
       </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27">
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>100</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>21</v>
       </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29">
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>110</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D29">
-        <v>3</v>
-      </c>
-      <c r="E29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31">
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>120</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>25</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>23</v>
       </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>130</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>29</v>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
       </c>
-      <c r="D34">
-        <v>3</v>
-      </c>
-      <c r="E34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>131</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>140</v>
       </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
         <v>24</v>
       </c>
-      <c r="D36">
-        <v>3</v>
-      </c>
-      <c r="E36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38">
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39">
         <v>150</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>27</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>28</v>
       </c>
-      <c r="D38">
-        <v>3</v>
-      </c>
-      <c r="E38">
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Setup instructions and Generation Log
</commit_message>
<xml_diff>
--- a/_workingFolder/CFBData/GenerationLog.xlsx
+++ b/_workingFolder/CFBData/GenerationLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuhnso\Documents\GitHub\StructuralEvaluationOfCFB\_workingFolder\CFBData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFC5076-C426-448F-92C1-EC2DA573D605}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9F362B-8601-4517-AE88-86D9F98EAC3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" activeTab="1" xr2:uid="{13CAE3C4-3EF5-4EF3-84E6-2C4B09A97B5A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
   <si>
     <t>Generation Log</t>
   </si>
@@ -166,16 +166,22 @@
     <t>L (2000,18000)</t>
   </si>
   <si>
-    <t>ibkiltis</t>
-  </si>
-  <si>
-    <t>&gt; after plot 520 521 comparison</t>
-  </si>
-  <si>
     <t>Hero Parameters (fsu_fac=1.08, d1/4_p/w=30, d3=20, t_p/w=700)</t>
   </si>
   <si>
     <t>ibkGuerza</t>
+  </si>
+  <si>
+    <t>idlWS2</t>
+  </si>
+  <si>
+    <t>ibkIltis</t>
+  </si>
+  <si>
+    <t>Error Files</t>
+  </si>
+  <si>
+    <t>0,1</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF7442-AE2A-41D1-AC75-AC2A4CC2EA55}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1019,12 +1025,12 @@
     <col min="3" max="3" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1049,8 +1055,11 @@
       <c r="H3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>501</v>
       </c>
@@ -1070,7 +1079,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>510</v>
       </c>
@@ -1090,7 +1099,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>520</v>
       </c>
@@ -1110,7 +1119,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>521</v>
       </c>
@@ -1127,15 +1136,13 @@
         <v>20</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>522</v>
       </c>
@@ -1152,10 +1159,13 @@
         <v>20</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>523</v>
       </c>
@@ -1172,10 +1182,12 @@
         <v>20</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>30</v>
       </c>
@@ -1192,7 +1204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>540</v>
       </c>
@@ -1210,10 +1222,13 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="J16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>541</v>
       </c>
@@ -1230,13 +1245,16 @@
         <v>20</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>542</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
@@ -1249,7 +1267,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>50</v>
       </c>
@@ -1266,7 +1284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>60</v>
       </c>
@@ -1283,7 +1301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>70</v>
       </c>
@@ -1300,7 +1318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>80</v>
       </c>
@@ -1317,7 +1335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>90</v>
       </c>
@@ -1334,7 +1352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>100</v>
       </c>
@@ -1351,7 +1369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>110</v>
       </c>

</xml_diff>